<commit_message>
Update excel and font
</commit_message>
<xml_diff>
--- a/Recipe_Database_Corrected.xlsx
+++ b/Recipe_Database_Corrected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taiyenwu/Downloads/Savor in the bay/github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB755331-7D9F-904A-9053-4AAD3F9DF519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F627DD-C9A3-8D4B-B948-E84EBB7153B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recipes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="125">
   <si>
     <t>RecipeID</t>
   </si>
@@ -314,6 +314,90 @@
   </si>
   <si>
     <t>https://i.imgur.com/myWJXK6.jpeg</t>
+  </si>
+  <si>
+    <t>R005</t>
+  </si>
+  <si>
+    <t>Korean Fried Chicken</t>
+  </si>
+  <si>
+    <t>韓式炸雞</t>
+  </si>
+  <si>
+    <t>5 ea</t>
+  </si>
+  <si>
+    <t>200C/400F</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TvxBgLp.jpeg</t>
+  </si>
+  <si>
+    <t>C008</t>
+  </si>
+  <si>
+    <t>C009</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>醬料</t>
+  </si>
+  <si>
+    <t>Chicken thigh</t>
+  </si>
+  <si>
+    <t>黑胡椒</t>
+  </si>
+  <si>
+    <t>Black pepper</t>
+  </si>
+  <si>
+    <t>Baking powder</t>
+  </si>
+  <si>
+    <t>白胡椒</t>
+  </si>
+  <si>
+    <t>White pepper</t>
+  </si>
+  <si>
+    <t>蜂蜜</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>韓式辣醬</t>
+  </si>
+  <si>
+    <t>Gochujang</t>
+  </si>
+  <si>
+    <t>番茄醬</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>雞腿</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>spoon</t>
+  </si>
+  <si>
+    <t>Green Oion</t>
+  </si>
+  <si>
+    <t>White sesame</t>
+  </si>
+  <si>
+    <t>白芝麻</t>
   </si>
 </sst>
 </file>
@@ -694,14 +778,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -835,16 +920,47 @@
         <v>94</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{0392B9BB-D452-5A4D-85B5-D70D33110A22}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -958,6 +1074,34 @@
       </c>
       <c r="D8" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -967,11 +1111,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1730,6 +1879,246 @@
         <v>71</v>
       </c>
       <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>121</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1740,9 +2129,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1930,6 +2321,70 @@
         <v>19</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update few new features
</commit_message>
<xml_diff>
--- a/Recipe_Database_Corrected.xlsx
+++ b/Recipe_Database_Corrected.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taiyenwu/Downloads/Savor in the bay/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taiyenwu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45F19A7-BA99-FF47-9E8A-2EBE5C604353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8646AFC-A289-7247-A4FD-C7C60BAA9AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,14 @@
     <sheet name="Components" sheetId="2" r:id="rId2"/>
     <sheet name="Ingredients" sheetId="3" r:id="rId3"/>
     <sheet name="IngredientDict" sheetId="4" r:id="rId4"/>
+    <sheet name="Steps" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="167">
   <si>
     <t>RecipeID</t>
   </si>
@@ -52,66 +53,96 @@
     <t>R001</t>
   </si>
   <si>
+    <t>Lemon Bar</t>
+  </si>
+  <si>
+    <t>檸檬方塊</t>
+  </si>
+  <si>
+    <t>1 ea</t>
+  </si>
+  <si>
+    <t>Bake</t>
+  </si>
+  <si>
+    <t>170C/340F</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QXCoWk0.jpeg</t>
+  </si>
+  <si>
     <t>R002</t>
   </si>
   <si>
+    <t>Scone</t>
+  </si>
+  <si>
+    <t>司康</t>
+  </si>
+  <si>
+    <t>6 ea</t>
+  </si>
+  <si>
+    <t>180C/360F</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/nzrstcI.jpeg</t>
+  </si>
+  <si>
     <t>R003</t>
   </si>
   <si>
+    <t>Caramel Custard</t>
+  </si>
+  <si>
+    <t>烤布丁</t>
+  </si>
+  <si>
+    <t>4 ea</t>
+  </si>
+  <si>
+    <t>130C/275F</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TIM3nkd.jpeg</t>
+  </si>
+  <si>
     <t>R004</t>
   </si>
   <si>
-    <t>Lemon Bar</t>
-  </si>
-  <si>
-    <t>Scone</t>
-  </si>
-  <si>
-    <t>Caramel Custard</t>
-  </si>
-  <si>
     <t>Strawberry Pei</t>
   </si>
   <si>
-    <t>檸檬方塊</t>
-  </si>
-  <si>
-    <t>司康</t>
-  </si>
-  <si>
-    <t>烤布丁</t>
-  </si>
-  <si>
     <t>莓果派</t>
   </si>
   <si>
-    <t>1 ea</t>
-  </si>
-  <si>
-    <t>6 ea</t>
-  </si>
-  <si>
-    <t>4 ea</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 ea </t>
   </si>
   <si>
-    <t>Bake</t>
-  </si>
-  <si>
-    <t>170C/340F</t>
-  </si>
-  <si>
-    <t>180C/360F</t>
-  </si>
-  <si>
-    <t>130C/275F</t>
-  </si>
-  <si>
     <t>220C/430F</t>
   </si>
   <si>
+    <t>https://i.imgur.com/BqFfyM1.jpeg</t>
+  </si>
+  <si>
+    <t>R005</t>
+  </si>
+  <si>
+    <t>Korean Fried Chicken</t>
+  </si>
+  <si>
+    <t>韓式炸雞</t>
+  </si>
+  <si>
+    <t>5 ea</t>
+  </si>
+  <si>
+    <t>200C/400F</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TvxBgLp.jpeg</t>
+  </si>
+  <si>
     <t>ComponentID</t>
   </si>
   <si>
@@ -124,52 +155,64 @@
     <t>C001</t>
   </si>
   <si>
+    <t>Pastry</t>
+  </si>
+  <si>
+    <t>餅皮</t>
+  </si>
+  <si>
     <t>C002</t>
   </si>
   <si>
+    <t>Filling</t>
+  </si>
+  <si>
+    <t>餡料</t>
+  </si>
+  <si>
     <t>C003</t>
   </si>
   <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>主體</t>
+  </si>
+  <si>
     <t>C004</t>
   </si>
   <si>
+    <t>Caramel</t>
+  </si>
+  <si>
+    <t>焦糖</t>
+  </si>
+  <si>
     <t>C005</t>
   </si>
   <si>
+    <t>Pudding</t>
+  </si>
+  <si>
+    <t>布丁</t>
+  </si>
+  <si>
     <t>C006</t>
   </si>
   <si>
     <t>C007</t>
   </si>
   <si>
-    <t>Pastry</t>
-  </si>
-  <si>
-    <t>Filling</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Caramel</t>
-  </si>
-  <si>
-    <t>Pudding</t>
-  </si>
-  <si>
-    <t>餅皮</t>
-  </si>
-  <si>
-    <t>餡料</t>
-  </si>
-  <si>
-    <t>主體</t>
-  </si>
-  <si>
-    <t>焦糖</t>
-  </si>
-  <si>
-    <t>布丁</t>
+    <t>C008</t>
+  </si>
+  <si>
+    <t>C009</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>醬料</t>
   </si>
   <si>
     <t>Ingredient</t>
@@ -187,6 +230,9 @@
     <t>All-purpose flour</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
     <t>Frozen Butter</t>
   </si>
   <si>
@@ -208,12 +254,18 @@
     <t>Egg</t>
   </si>
   <si>
+    <t>ea</t>
+  </si>
+  <si>
     <t>Baking Soda</t>
   </si>
   <si>
     <t>Milk</t>
   </si>
   <si>
+    <t>ml</t>
+  </si>
+  <si>
     <t>Yolk</t>
   </si>
   <si>
@@ -238,13 +290,37 @@
     <t>Blueberry</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>ml</t>
+    <t>Chicken thigh</t>
+  </si>
+  <si>
+    <t>Black pepper</t>
+  </si>
+  <si>
+    <t>Baking powder</t>
+  </si>
+  <si>
+    <t>White pepper</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>spoon</t>
+  </si>
+  <si>
+    <t>Gochujang</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Green Oion</t>
+  </si>
+  <si>
+    <t>White sesame</t>
   </si>
   <si>
     <t>Ingredient_zh</t>
@@ -304,100 +380,151 @@
     <t>蛋黃</t>
   </si>
   <si>
-    <t>https://i.imgur.com/QXCoWk0.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/BqFfyM1.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/TIM3nkd.jpeg</t>
-  </si>
-  <si>
-    <t>R005</t>
-  </si>
-  <si>
-    <t>Korean Fried Chicken</t>
-  </si>
-  <si>
-    <t>韓式炸雞</t>
-  </si>
-  <si>
-    <t>5 ea</t>
-  </si>
-  <si>
-    <t>200C/400F</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/TvxBgLp.jpeg</t>
-  </si>
-  <si>
-    <t>C008</t>
-  </si>
-  <si>
-    <t>C009</t>
-  </si>
-  <si>
-    <t>Sauce</t>
-  </si>
-  <si>
-    <t>醬料</t>
-  </si>
-  <si>
-    <t>Chicken thigh</t>
+    <t>雞腿</t>
   </si>
   <si>
     <t>黑胡椒</t>
   </si>
   <si>
-    <t>Black pepper</t>
-  </si>
-  <si>
-    <t>Baking powder</t>
-  </si>
-  <si>
     <t>白胡椒</t>
   </si>
   <si>
-    <t>White pepper</t>
-  </si>
-  <si>
     <t>蜂蜜</t>
   </si>
   <si>
-    <t>Honey</t>
-  </si>
-  <si>
     <t>韓式辣醬</t>
   </si>
   <si>
-    <t>Gochujang</t>
-  </si>
-  <si>
     <t>番茄醬</t>
   </si>
   <si>
-    <t>Ketchup</t>
-  </si>
-  <si>
-    <t>雞腿</t>
-  </si>
-  <si>
-    <t>Garlic</t>
-  </si>
-  <si>
-    <t>spoon</t>
-  </si>
-  <si>
-    <t>Green Oion</t>
-  </si>
-  <si>
-    <t>White sesame</t>
-  </si>
-  <si>
     <t>白芝麻</t>
   </si>
   <si>
-    <t>https://i.imgur.com/nzrstcI.jpeg</t>
+    <t>StepOrder</t>
+  </si>
+  <si>
+    <t>Instruction_en</t>
+  </si>
+  <si>
+    <t>Instruction_zh</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Category_zh</t>
+  </si>
+  <si>
+    <t>Dessert</t>
+  </si>
+  <si>
+    <t>Main Course</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>SubCategory_zh</t>
+  </si>
+  <si>
+    <t>European-style</t>
+  </si>
+  <si>
+    <t>American-style</t>
+  </si>
+  <si>
+    <t>Japanese-style</t>
+  </si>
+  <si>
+    <t>Korean-style</t>
+  </si>
+  <si>
+    <t>美式</t>
+  </si>
+  <si>
+    <t>歐式</t>
+  </si>
+  <si>
+    <t>日式</t>
+  </si>
+  <si>
+    <t>韓式</t>
+  </si>
+  <si>
+    <t>點心</t>
+  </si>
+  <si>
+    <t>主菜</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Part_zh</t>
+  </si>
+  <si>
+    <t>Crust</t>
+  </si>
+  <si>
+    <t>裝飾</t>
+  </si>
+  <si>
+    <t>Decoration</t>
+  </si>
+  <si>
+    <t>將烤模塗上奶油，然後鋪上烘焙紙。</t>
+  </si>
+  <si>
+    <t>將中筋麵粉過篩，與冷凍奶油、糖粉和鹽一起放入料理機中，打碎成砂礫狀。</t>
+  </si>
+  <si>
+    <t>將混合物倒入烤模中，壓平，並用叉子在表面戳出一些小洞，以便後續餡料滲入。</t>
+  </si>
+  <si>
+    <t>將烤模放入烤箱，以170°C烘烤約22分鐘。</t>
+  </si>
+  <si>
+    <t>將奶油、檸檬汁、糖和雞蛋混合攪拌均勻，表面的氣泡可用餐巾紙吸附去除。</t>
+  </si>
+  <si>
+    <t>將攪拌好的餡料倒入烤好的餅皮模具中。</t>
+  </si>
+  <si>
+    <t>將模具再次放入烤箱，以170°C烘烤約10分鐘。</t>
+  </si>
+  <si>
+    <t>烤好後，刨上檸檬屑，並用喜歡的水果裝飾。</t>
+  </si>
+  <si>
+    <t>Grease the baking mold with butter and line it with parchment paper.</t>
+  </si>
+  <si>
+    <t>Sift the all-purpose flour and place it in a food processor with frozen butter, powdered sugar, and salt. Process until the mixture resembles coarse crumbs.</t>
+  </si>
+  <si>
+    <t>Pour the mixture into the baking mold, press it flat, and poke holes on the surface with a fork to allow the filling to penetrate later.</t>
+  </si>
+  <si>
+    <t>Bake in the oven at 170°C (340°F) for about 22 minutes.</t>
+  </si>
+  <si>
+    <t>Mix butter, lemon juice, sugar, and eggs until well combined. Remove any surface bubbles by dabbing with a paper towel.</t>
+  </si>
+  <si>
+    <t>Pour the filling into the baked crust in the mold.</t>
+  </si>
+  <si>
+    <t>Bake again in the oven at 170°C (340°F) for about 10 minutes.</t>
+  </si>
+  <si>
+    <t>After baking, sprinkle with lemon zest and decorate with your favorite fruits.</t>
+  </si>
+  <si>
+    <t>CycleTime</t>
+  </si>
+  <si>
+    <t>Parallel</t>
   </si>
 </sst>
 </file>
@@ -415,17 +542,16 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,7 +562,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -459,23 +585,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,9 +633,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -532,7 +673,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -566,7 +707,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -601,10 +741,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -778,19 +917,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,142 +957,214 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{0392B9BB-D452-5A4D-85B5-D70D33110A22}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -958,35 +1172,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
@@ -994,69 +1206,69 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1064,48 +1276,48 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1113,33 +1325,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1147,16 +1356,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D2">
         <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -1167,16 +1376,16 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1187,16 +1396,16 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1207,16 +1416,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1227,16 +1436,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1247,16 +1456,16 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1267,16 +1476,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1287,16 +1496,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1304,19 +1513,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D10">
         <v>210</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1324,19 +1533,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D11">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1344,19 +1553,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D12">
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1364,19 +1573,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D13">
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1384,19 +1593,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1404,19 +1613,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1424,19 +1633,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>0.5</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1444,19 +1653,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1464,19 +1673,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D18">
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1484,19 +1693,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D19">
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1504,19 +1713,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D20">
         <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1524,19 +1733,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D21">
         <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1544,19 +1753,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1564,19 +1773,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D23">
         <v>200</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1584,19 +1793,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D24">
         <v>140</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1604,19 +1813,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -1624,19 +1833,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1644,19 +1853,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1664,19 +1873,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D28">
         <v>150</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1684,19 +1893,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D29">
         <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1704,19 +1913,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D30">
         <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1724,19 +1933,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1744,19 +1953,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D32">
         <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1764,19 +1973,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1784,19 +1993,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D34">
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1804,19 +2013,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D35">
         <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1824,19 +2033,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>0.5</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1844,19 +2053,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D37">
         <v>200</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1864,19 +2073,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D38">
         <v>40</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1884,19 +2093,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1904,19 +2113,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -1924,19 +2133,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="D41">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -1944,19 +2153,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -1964,19 +2173,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -1984,19 +2193,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="D44">
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -2004,19 +2213,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D45">
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -2024,19 +2233,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -2044,19 +2253,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -2064,19 +2273,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
         <v>96</v>
-      </c>
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" t="s">
-        <v>117</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -2084,19 +2293,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2104,26 +2313,26 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2131,175 +2340,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -2307,23 +2514,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
         <v>118</v>
@@ -2331,61 +2538,327 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="118.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="63.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="60.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="4">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="4">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>